<commit_message>
Fixed the first row for easy review.
</commit_message>
<xml_diff>
--- a/models/gov.us.fhim/reports/FHIM Behavioral Health Domain - Classes.xlsx
+++ b/models/gov.us.fhim/reports/FHIM Behavioral Health Domain - Classes.xlsx
@@ -1369,16 +1369,17 @@
   <dimension ref="A1:G149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="51.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
@@ -1525,7 +1526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="51">
+    <row r="8" spans="1:7" ht="38.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1698,7 +1699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="63.75">
+    <row r="17" spans="1:7" ht="51">
       <c r="A17" s="5" t="s">
         <v>39</v>
       </c>
@@ -1753,7 +1754,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="38.25">
+    <row r="20" spans="1:7" ht="25.5">
       <c r="A20" s="5" t="s">
         <v>55</v>
       </c>
@@ -1774,7 +1775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="51">
+    <row r="21" spans="1:7" ht="38.25">
       <c r="A21" s="5" t="s">
         <v>55</v>
       </c>
@@ -2225,7 +2226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="38.25">
+    <row r="46" spans="1:7" ht="25.5">
       <c r="A46" s="5" t="s">
         <v>113</v>
       </c>
@@ -2244,7 +2245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="38.25">
+    <row r="47" spans="1:7" ht="25.5">
       <c r="A47" s="5" t="s">
         <v>113</v>
       </c>
@@ -2554,7 +2555,7 @@
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
     </row>
-    <row r="65" spans="1:7" ht="25.5">
+    <row r="65" spans="1:7">
       <c r="A65" s="5" t="s">
         <v>80</v>
       </c>
@@ -2573,7 +2574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="25.5">
+    <row r="66" spans="1:7">
       <c r="A66" s="5" t="s">
         <v>80</v>
       </c>
@@ -2592,7 +2593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="38.25">
+    <row r="67" spans="1:7" ht="25.5">
       <c r="A67" s="5" t="s">
         <v>80</v>
       </c>
@@ -2624,7 +2625,7 @@
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
     </row>
-    <row r="69" spans="1:7" ht="25.5">
+    <row r="69" spans="1:7">
       <c r="A69" s="5" t="s">
         <v>161</v>
       </c>
@@ -2656,7 +2657,7 @@
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
     </row>
-    <row r="71" spans="1:7" ht="38.25">
+    <row r="71" spans="1:7" ht="25.5">
       <c r="A71" s="5" t="s">
         <v>164</v>
       </c>
@@ -2824,7 +2825,7 @@
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
     </row>
-    <row r="81" spans="1:7" ht="25.5">
+    <row r="81" spans="1:7">
       <c r="A81" s="5" t="s">
         <v>52</v>
       </c>
@@ -3099,7 +3100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="51">
+    <row r="96" spans="1:7" ht="38.25">
       <c r="A96" s="5" t="s">
         <v>25</v>
       </c>
@@ -3306,7 +3307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="38.25">
+    <row r="107" spans="1:7" ht="25.5">
       <c r="A107" s="5" t="s">
         <v>28</v>
       </c>
@@ -3452,7 +3453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="25.5">
+    <row r="115" spans="1:7">
       <c r="A115" s="5" t="s">
         <v>238</v>
       </c>
@@ -3634,7 +3635,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="51">
+    <row r="125" spans="1:7" ht="38.25">
       <c r="A125" s="5" t="s">
         <v>218</v>
       </c>
@@ -3666,7 +3667,7 @@
       <c r="F126" s="4"/>
       <c r="G126" s="4"/>
     </row>
-    <row r="127" spans="1:7" ht="25.5">
+    <row r="127" spans="1:7">
       <c r="A127" s="5" t="s">
         <v>271</v>
       </c>
@@ -3685,7 +3686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="38.25">
+    <row r="128" spans="1:7" ht="25.5">
       <c r="A128" s="5" t="s">
         <v>271</v>
       </c>
@@ -3904,7 +3905,7 @@
       <c r="F140" s="4"/>
       <c r="G140" s="4"/>
     </row>
-    <row r="141" spans="1:7" ht="38.25">
+    <row r="141" spans="1:7" ht="25.5">
       <c r="A141" s="5" t="s">
         <v>288</v>
       </c>
@@ -3957,7 +3958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="25.5">
+    <row r="144" spans="1:7">
       <c r="A144" s="5" t="s">
         <v>281</v>
       </c>

</xml_diff>